<commit_message>
refactor: Remove farmerName placeholder from farmer invitation SMS templates
Removed {farmerName} placeholder from both single and bulk farmer invitation handlers.
Template now uses only: {sponsorName}, {playStoreLink}, {expiryDays}

Changes:
- CreateFarmerInvitationCommand.cs: Removed .Replace("{farmerName}", ...)
- BulkCreateFarmerInvitationsCommand.cs: Removed .Replace("{farmerName}", ...)

This aligns with user requirement to not include farmerName in SMS template.

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/claudedocs/Farmers/Farmer_Invitations_Bulk_Upload_Template.xlsx
+++ b/claudedocs/Farmers/Farmer_Invitations_Bulk_Upload_Template.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Documents\Visual Studio 2022\ziraai\claudedocs\Farmers\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Farmer Invitations" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Phone</t>
   </si>
@@ -31,18 +36,12 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>05551234567</t>
-  </si>
-  <si>
     <t>Ahmet Yılmaz</t>
   </si>
   <si>
     <t>ahmet@example.com</t>
   </si>
   <si>
-    <t>M</t>
-  </si>
-  <si>
     <t>İlk davet</t>
   </si>
   <si>
@@ -52,9 +51,6 @@
     <t>Mehmet Demir</t>
   </si>
   <si>
-    <t>S</t>
-  </si>
-  <si>
     <t>Küçük üretici</t>
   </si>
   <si>
@@ -67,9 +63,6 @@
     <t>ayse@email.com</t>
   </si>
   <si>
-    <t>L</t>
-  </si>
-  <si>
     <t>Premium müşteri</t>
   </si>
   <si>
@@ -91,17 +84,17 @@
     <t>Ali Yıldız</t>
   </si>
   <si>
-    <t>XL</t>
-  </si>
-  <si>
     <t>VIP çiftçi</t>
+  </si>
+  <si>
+    <t>05069468693</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -159,12 +152,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -173,11 +169,19 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Teması">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -219,7 +223,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -251,9 +255,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -285,6 +290,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -460,15 +466,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.7109375" customWidth="1"/>
     <col min="2" max="2" width="18.7109375" customWidth="1"/>
@@ -477,7 +483,7 @@
     <col min="5" max="5" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -494,86 +500,79 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2"/>
+      <c r="E2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="2" t="s">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="2" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2" t="s">
+      <c r="B4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="2" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="B5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="2" t="s">
-        <v>23</v>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C6" s="2"/>
-      <c r="D6" s="2" t="s">
-        <v>25</v>
-      </c>
+      <c r="D6" s="2"/>
       <c r="E6" s="2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>